<commit_message>
tic tac toe working
</commit_message>
<xml_diff>
--- a/sudoku Q1.xlsx
+++ b/sudoku Q1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="840" windowWidth="16860" windowHeight="13620"/>
+    <workbookView xWindow="11940" yWindow="960" windowWidth="16860" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,10 +480,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -506,8 +522,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -515,7 +535,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -817,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -835,9 +859,13 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <f>SUM(B3:B127)</f>
+        <v>13.782119999999999</v>
+      </c>
       <c r="C2">
-        <f>SUM(B:B)</f>
-        <v>13.782119999999999</v>
+        <f>SUM(C3:C117)</f>
+        <v>869841</v>
       </c>
       <c r="E2" t="s">
         <v>130</v>

</xml_diff>